<commit_message>
raw: primeiras tabelas dimensão criadas
</commit_message>
<xml_diff>
--- a/Docs/Doc Schema.xlsx
+++ b/Docs/Doc Schema.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bungeltd.sharepoint.com/sites/DadosSupplyOrigeo/Shared Documents/Projeto_Dados/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E464B6F-7A2C-4ED0-BA17-39E380ED5DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="8_{2E464B6F-7A2C-4ED0-BA17-39E380ED5DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E6F15CC-3133-4C5F-935E-D79563CA1FE3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CBF119E8-B3C9-4986-8153-C47CD5816AE1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Extraction" sheetId="1" r:id="rId1"/>
-    <sheet name="Transform" sheetId="2" r:id="rId2"/>
+    <sheet name="DataFrame" sheetId="1" r:id="rId1"/>
+    <sheet name="DataLake" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
   <si>
     <t>Source</t>
   </si>
@@ -75,46 +75,79 @@
     <t>str</t>
   </si>
   <si>
-    <t>Contrato Venda</t>
-  </si>
-  <si>
-    <t>Item Contrato</t>
-  </si>
-  <si>
-    <t>Pedido SalesForce</t>
-  </si>
-  <si>
-    <t>Tipo Documento</t>
-  </si>
-  <si>
-    <t>Data de criação</t>
-  </si>
-  <si>
-    <t>Data Início Entrega</t>
-  </si>
-  <si>
-    <t>Data Fim Entrega</t>
-  </si>
-  <si>
-    <t>Qtde Contrato</t>
-  </si>
-  <si>
-    <t>Valor Contrato</t>
-  </si>
-  <si>
-    <t>Moeda</t>
-  </si>
-  <si>
-    <t>Id Mot. Rec.</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
     <t>FK</t>
+  </si>
+  <si>
+    <t>Centro</t>
+  </si>
+  <si>
+    <t>CNPJ</t>
+  </si>
+  <si>
+    <t>Nível 2</t>
+  </si>
+  <si>
+    <t>Nível 1</t>
+  </si>
+  <si>
+    <t>UF</t>
+  </si>
+  <si>
+    <t>Local Expedição</t>
+  </si>
+  <si>
+    <t>Id UF</t>
+  </si>
+  <si>
+    <t>Cidade</t>
+  </si>
+  <si>
+    <t>Id Cidade</t>
+  </si>
+  <si>
+    <t>Nível 3</t>
+  </si>
+  <si>
+    <t>Motivo Recusa</t>
+  </si>
+  <si>
+    <t>Zona Transporte</t>
+  </si>
+  <si>
+    <t>Nível 4</t>
+  </si>
+  <si>
+    <t>Id Zona Transp</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>CNPJ Raiz</t>
+  </si>
+  <si>
+    <t>CPF</t>
+  </si>
+  <si>
+    <t>Ins Est</t>
+  </si>
+  <si>
+    <t>Ins Mun</t>
+  </si>
+  <si>
+    <t>Nível 5</t>
+  </si>
+  <si>
+    <t>Itinerário</t>
+  </si>
+  <si>
+    <t>Distância</t>
+  </si>
+  <si>
+    <t>Id Local Exp</t>
+  </si>
+  <si>
+    <t>Id Cliente</t>
   </si>
 </sst>
 </file>
@@ -145,7 +178,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +194,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,10 +296,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -271,14 +309,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -300,23 +346,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1171575</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Conector de Seta Reta 2">
+        <xdr:cNvPr id="6" name="Conector de Seta Reta 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{419D7E4A-819F-F96B-CAB3-9E13054A742A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84EF462B-E97E-4749-98C1-F1F91031771B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -324,8 +370,288 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1447800" y="466725"/>
-          <a:ext cx="3238500" cy="1743075"/>
+          <a:off x="3190875" y="914400"/>
+          <a:ext cx="2400300" cy="95250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Conector de Seta Reta 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84CCCC0F-F38D-82C9-C393-22BBCE2BF0BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="838200" y="838200"/>
+          <a:ext cx="2057400" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1171575</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Conector de Seta Reta 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04D57EDA-2EAE-40FD-80A6-A08A270B19DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6029325" y="895350"/>
+          <a:ext cx="2409825" cy="2390775"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Conector de Seta Reta 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B2FDB6C-B268-4DFA-AE10-FF4A8D29A8C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5924550" y="933450"/>
+          <a:ext cx="2562225" cy="4362450"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Conector de Seta Reta 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DBE88D4-9B5F-44E3-B6C1-59046D29A7CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8848725" y="1466850"/>
+          <a:ext cx="2009775" cy="1438275"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Conector de Seta Reta 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B54C4C9-F357-49AE-B7BE-C129BAE521B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8810625" y="1619250"/>
+          <a:ext cx="2286000" cy="2571750"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -560,7 +886,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2996D40E-876F-400F-9F12-57E2C35E6BCD}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -568,25 +894,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1" hidden="1"/>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -633,169 +959,458 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01925E2E-6FB2-4848-9825-FD424C1ED897}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="E1" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="I1" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="M1" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="Q1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+      <c r="I3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="4"/>
+      <c r="M3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="4"/>
+      <c r="Q3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="3"/>
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="R5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="N6" s="11"/>
+      <c r="O6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R6" s="15"/>
+      <c r="S6" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" s="15"/>
+      <c r="S7" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="E8" s="13"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="M8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="3"/>
+      <c r="O8" s="4"/>
+      <c r="Q8" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="R8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="N9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="O9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="Q9" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="S9" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="M10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="M11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" s="15"/>
+      <c r="O11" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12" s="11"/>
+      <c r="O12" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="M14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="3"/>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="M15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="N15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="O15" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="M16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="N16" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="9" t="s">
+      <c r="O16" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="M17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17" s="15"/>
+      <c r="O17" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="M18" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="N18" s="15"/>
+      <c r="O18" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="13:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M19" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="N19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="O19" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="13:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M20" s="13"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+    </row>
+    <row r="21" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="M21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N21" s="3"/>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="22" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="M22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N22" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="M23" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N23" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="O23" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="11" t="s">
+    <row r="24" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="M24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N24" s="15"/>
+      <c r="O24" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="M25" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="N25" s="15"/>
+      <c r="O25" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E5" s="9" t="s">
+    <row r="26" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="M26" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="14" t="s">
+      <c r="N26" s="15"/>
+      <c r="O26" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="M27" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="N27" s="15"/>
+      <c r="O27" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="M28" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="N28" s="15"/>
+      <c r="O28" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="M29" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="N29" s="15"/>
+      <c r="O29" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="13:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M30" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O30" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -983,6 +1598,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -991,22 +1612,40 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C36481A5-65FA-43B5-9936-42D393C8166C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C36481A5-65FA-43B5-9936-42D393C8166C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a23e95a4-e77e-4c3b-9a33-dadacf3bd6c1"/>
+    <ds:schemaRef ds:uri="c6efae78-7c8a-4441-a198-ae3f040086cd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EF9DAF2-2BB7-423F-B396-DB7EFC3ABE13}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39FBB235-1553-4865-A28D-01E1A5E87283}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39FBB235-1553-4865-A28D-01E1A5E87283}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EF9DAF2-2BB7-423F-B396-DB7EFC3ABE13}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
fix: ajustando relacionamento entre tabelas
</commit_message>
<xml_diff>
--- a/Docs/Doc Schema.xlsx
+++ b/Docs/Doc Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bungeltd.sharepoint.com/sites/DadosSupplyOrigeo/Shared Documents/Projeto_Dados/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="167" documentId="8_{2E464B6F-7A2C-4ED0-BA17-39E380ED5DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E6F15CC-3133-4C5F-935E-D79563CA1FE3}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="8_{2E464B6F-7A2C-4ED0-BA17-39E380ED5DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9F1FC7B-4FE0-416A-8C41-AEF11F2E16E4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CBF119E8-B3C9-4986-8153-C47CD5816AE1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="36">
   <si>
     <t>Source</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Motivo Recusa</t>
   </si>
   <si>
-    <t>Zona Transporte</t>
-  </si>
-  <si>
     <t>Nível 4</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>Ins Mun</t>
   </si>
   <si>
-    <t>Nível 5</t>
-  </si>
-  <si>
     <t>Itinerário</t>
   </si>
   <si>
@@ -148,6 +142,9 @@
   </si>
   <si>
     <t>Id Cliente</t>
+  </si>
+  <si>
+    <t>Zona Transp</t>
   </si>
 </sst>
 </file>
@@ -296,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -316,14 +313,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -344,62 +341,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Conector de Seta Reta 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84EF462B-E97E-4749-98C1-F1F91031771B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3190875" y="914400"/>
-          <a:ext cx="2400300" cy="95250"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -458,16 +399,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>302560</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>83484</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1171575</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1154206</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -482,8 +423,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6029325" y="895350"/>
-          <a:ext cx="2409825" cy="2390775"/>
+          <a:off x="3216089" y="800660"/>
+          <a:ext cx="2409264" cy="712134"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -514,23 +455,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>186</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1219200</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1131794</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>145677</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="23" name="Conector de Seta Reta 22">
+        <xdr:cNvPr id="19" name="Conector de Seta Reta 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B2FDB6C-B268-4DFA-AE10-FF4A8D29A8C6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC791439-428B-4CC6-B588-3A2992341C97}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -538,120 +479,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5924550" y="933450"/>
-          <a:ext cx="2562225" cy="4362450"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="25" name="Conector de Seta Reta 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DBE88D4-9B5F-44E3-B6C1-59046D29A7CA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8848725" y="1466850"/>
-          <a:ext cx="2009775" cy="1438275"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="27" name="Conector de Seta Reta 26">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B54C4C9-F357-49AE-B7BE-C129BAE521B0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8810625" y="1619250"/>
-          <a:ext cx="2286000" cy="2571750"/>
+          <a:off x="3104030" y="896657"/>
+          <a:ext cx="2498911" cy="3014196"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -892,15 +721,15 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" hidden="1"/>
+    <col min="1" max="1" width="8.84375" customWidth="1"/>
+    <col min="2" max="2" width="12.4609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.84375" customWidth="1"/>
+    <col min="4" max="16384" width="8.84375" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -908,7 +737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -916,42 +745,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="17" x14ac:dyDescent="0.2"/>
-    <row r="18" x14ac:dyDescent="0.2"/>
-    <row r="19" x14ac:dyDescent="0.2"/>
-    <row r="20" x14ac:dyDescent="0.2"/>
-    <row r="21" x14ac:dyDescent="0.2"/>
-    <row r="22" x14ac:dyDescent="0.2"/>
-    <row r="23" x14ac:dyDescent="0.2"/>
-    <row r="24" x14ac:dyDescent="0.2"/>
-    <row r="25" x14ac:dyDescent="0.2"/>
-    <row r="26" x14ac:dyDescent="0.2"/>
-    <row r="27" x14ac:dyDescent="0.2"/>
-    <row r="28" x14ac:dyDescent="0.2"/>
-    <row r="29" x14ac:dyDescent="0.2"/>
-    <row r="30" x14ac:dyDescent="0.2"/>
-    <row r="31" x14ac:dyDescent="0.2"/>
-    <row r="32" x14ac:dyDescent="0.2"/>
-    <row r="33" x14ac:dyDescent="0.2"/>
-    <row r="34" x14ac:dyDescent="0.2"/>
-    <row r="35" x14ac:dyDescent="0.2"/>
-    <row r="36" x14ac:dyDescent="0.2"/>
-    <row r="37" x14ac:dyDescent="0.2"/>
-    <row r="38" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="17" x14ac:dyDescent="0.3"/>
+    <row r="18" x14ac:dyDescent="0.3"/>
+    <row r="19" x14ac:dyDescent="0.3"/>
+    <row r="20" x14ac:dyDescent="0.3"/>
+    <row r="21" x14ac:dyDescent="0.3"/>
+    <row r="22" x14ac:dyDescent="0.3"/>
+    <row r="23" x14ac:dyDescent="0.3"/>
+    <row r="24" x14ac:dyDescent="0.3"/>
+    <row r="25" x14ac:dyDescent="0.3"/>
+    <row r="26" x14ac:dyDescent="0.3"/>
+    <row r="27" x14ac:dyDescent="0.3"/>
+    <row r="28" x14ac:dyDescent="0.3"/>
+    <row r="29" x14ac:dyDescent="0.3"/>
+    <row r="30" x14ac:dyDescent="0.3"/>
+    <row r="31" x14ac:dyDescent="0.3"/>
+    <row r="32" x14ac:dyDescent="0.3"/>
+    <row r="33" x14ac:dyDescent="0.3"/>
+    <row r="34" x14ac:dyDescent="0.3"/>
+    <row r="35" x14ac:dyDescent="0.3"/>
+    <row r="36" x14ac:dyDescent="0.3"/>
+    <row r="37" x14ac:dyDescent="0.3"/>
+    <row r="38" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -959,58 +788,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01925E2E-6FB2-4848-9825-FD424C1ED897}">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.69140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.84375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.69140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.53515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.84375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.69140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="E1" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="I1" s="19" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="E1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="M1" s="19" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="I1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="Q1" s="19" t="s">
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="M1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+    </row>
+    <row r="2" spans="1:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1022,22 +843,17 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
       <c r="I3" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="4"/>
       <c r="M3" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="4"/>
-      <c r="Q3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" s="3"/>
-      <c r="S3" s="4"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1050,7 +866,7 @@
       <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="7" t="s">
@@ -1059,7 +875,7 @@
       <c r="I4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="7" t="s">
@@ -1074,17 +890,8 @@
       <c r="O4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="R4" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
@@ -1097,16 +904,16 @@
       <c r="E5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
         <v>6</v>
       </c>
       <c r="K5" s="9" t="s">
@@ -1121,17 +928,8 @@
       <c r="O5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="R5" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="S5" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>17</v>
       </c>
@@ -1142,36 +940,24 @@
       <c r="E6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="15"/>
       <c r="G6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="N6" s="11"/>
-      <c r="O6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="R6" s="15"/>
-      <c r="S6" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="16" t="s">
+      <c r="I6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="11" t="s">
@@ -1180,237 +966,261 @@
       <c r="G7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q7" s="20" t="s">
+      <c r="I7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="I9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="R7" s="15"/>
-      <c r="S7" s="21" t="s">
+      <c r="N9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="16"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="I10" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="M11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="I12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="4"/>
+      <c r="M12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="I13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="E8" s="13"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="M8" s="2" t="s">
+      <c r="M14" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="N14" s="11"/>
+      <c r="O14" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="3"/>
-      <c r="O8" s="4"/>
-      <c r="Q8" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="R8" s="15" t="s">
+      <c r="N16" s="3"/>
+      <c r="O16" s="4"/>
+    </row>
+    <row r="17" spans="9:15" x14ac:dyDescent="0.3">
+      <c r="I17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="9:15" x14ac:dyDescent="0.3">
+      <c r="I18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N18" t="s">
+        <v>6</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="9:15" x14ac:dyDescent="0.3">
+      <c r="I19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="9:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="N20" s="11"/>
+      <c r="O20" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="9:15" x14ac:dyDescent="0.3">
+      <c r="I21" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" t="s">
         <v>12</v>
       </c>
-      <c r="S8" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="N9" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q9" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="R9" s="11" t="s">
+      <c r="K21" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="9:15" x14ac:dyDescent="0.3">
+      <c r="I22" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" t="s">
         <v>12</v>
       </c>
-      <c r="S9" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="M10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="N10" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="O10" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="M11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="N11" s="15"/>
-      <c r="O11" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M12" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="N12" s="11"/>
-      <c r="O12" s="17" t="s">
+      <c r="K22" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="M14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="4"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="M15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="N15" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="O15" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="M16" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="N16" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="O16" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="M17" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N17" s="15"/>
-      <c r="O17" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="M18" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="N18" s="15"/>
-      <c r="O18" s="21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="13:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M19" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="N19" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="O19" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="13:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M20" s="13"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-    </row>
-    <row r="21" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="M21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N21" s="3"/>
-      <c r="O21" s="4"/>
-    </row>
-    <row r="22" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="M22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="N22" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="O22" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="M23" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="N23" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="O23" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="M24" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N24" s="15"/>
-      <c r="O24" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="M25" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="N25" s="15"/>
-      <c r="O25" s="21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="M26" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="N26" s="15"/>
-      <c r="O26" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="M27" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="N27" s="15"/>
-      <c r="O27" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="M28" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="N28" s="15"/>
-      <c r="O28" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="13:15" x14ac:dyDescent="0.2">
-      <c r="M29" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="N29" s="15"/>
-      <c r="O29" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="13:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M30" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="N30" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="O30" s="12" t="s">
+    <row r="23" spans="9:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I23" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" s="11"/>
+      <c r="K23" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1598,18 +1408,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1632,18 +1442,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39FBB235-1553-4865-A28D-01E1A5E87283}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EF9DAF2-2BB7-423F-B396-DB7EFC3ABE13}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EF9DAF2-2BB7-423F-B396-DB7EFC3ABE13}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39FBB235-1553-4865-A28D-01E1A5E87283}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
build: DT e Conta Frete
</commit_message>
<xml_diff>
--- a/Docs/Doc Schema.xlsx
+++ b/Docs/Doc Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bungeltd.sharepoint.com/sites/DadosSupplyOrigeo/Shared Documents/Projeto_Dados/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="480" documentId="8_{2E464B6F-7A2C-4ED0-BA17-39E380ED5DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{057BC266-8651-4B31-B99D-CC24697F1ABE}"/>
+  <xr:revisionPtr revIDLastSave="539" documentId="8_{2E464B6F-7A2C-4ED0-BA17-39E380ED5DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B6E04AF-8C74-4C0D-84CA-09052DA2D19C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{CBF119E8-B3C9-4986-8153-C47CD5816AE1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="96">
   <si>
     <t>Source</t>
   </si>
@@ -292,6 +292,39 @@
   </si>
   <si>
     <t>datatime</t>
+  </si>
+  <si>
+    <t>Categoria DT</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Transportador</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>Nível 6</t>
+  </si>
+  <si>
+    <t>Valor Frete</t>
+  </si>
+  <si>
+    <t>Id Categoria</t>
+  </si>
+  <si>
+    <t>Id Transportador</t>
+  </si>
+  <si>
+    <t>Id NF</t>
+  </si>
+  <si>
+    <t>Conta Frete</t>
+  </si>
+  <si>
+    <t>Frete Pedido</t>
   </si>
 </sst>
 </file>
@@ -440,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -464,7 +497,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,7 +724,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -723,8 +759,22 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+    </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3"/>
@@ -765,28 +815,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01925E2E-6FB2-4848-9825-FD424C1ED897}">
-  <dimension ref="A1:W48"/>
+  <dimension ref="A1:AA48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.84375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.69140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.84375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.61328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.53515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.3046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.765625" customWidth="1"/>
-    <col min="13" max="13" width="14.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.53515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.15234375" customWidth="1"/>
+    <col min="13" max="13" width="15.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.921875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.4609375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.921875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.4609375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.921875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.3828125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.921875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -796,28 +859,33 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
       <c r="I1" s="14" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="J1" s="13"/>
       <c r="K1" s="13"/>
       <c r="M1" s="14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
       <c r="Q1" s="14" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="R1" s="13"/>
       <c r="S1" s="13"/>
       <c r="U1" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="V1" s="13"/>
       <c r="W1" s="13"/>
-    </row>
-    <row r="2" spans="1:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Y1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+    </row>
+    <row r="2" spans="1:27" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -848,8 +916,13 @@
       </c>
       <c r="V3" s="3"/>
       <c r="W3" s="4"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Y3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="4"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -898,14 +971,23 @@
       <c r="U4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="V4" s="15" t="s">
+      <c r="V4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="W4" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Y4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA4" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
@@ -954,14 +1036,23 @@
       <c r="U5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="V5" s="16" t="s">
+      <c r="V5" t="s">
         <v>6</v>
       </c>
       <c r="W5" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Y5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA5" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>17</v>
       </c>
@@ -997,14 +1088,21 @@
       <c r="U6" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="V6" s="16" t="s">
+      <c r="V6" t="s">
         <v>12</v>
       </c>
       <c r="W6" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Y6" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E7" s="10" t="s">
         <v>19</v>
       </c>
@@ -1029,14 +1127,21 @@
       <c r="U7" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="V7" s="16" t="s">
+      <c r="V7" t="s">
         <v>12</v>
       </c>
       <c r="W7" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Y7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1063,12 +1168,18 @@
       <c r="U8" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="V8" s="16"/>
       <c r="W8" s="9" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Y8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z8" s="16"/>
+      <c r="AA8" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="E9" s="2" t="s">
         <v>39</v>
       </c>
@@ -1098,12 +1209,18 @@
       <c r="U9" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="V9" s="16"/>
       <c r="W9" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Y9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z9" s="16"/>
+      <c r="AA9" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1137,12 +1254,18 @@
       <c r="U10" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="V10" s="16"/>
       <c r="W10" s="9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Y10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z10" s="16"/>
+      <c r="AA10" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="E11" s="8" t="s">
         <v>5</v>
       </c>
@@ -1173,12 +1296,18 @@
       <c r="U11" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="V11" s="16"/>
       <c r="W11" s="9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Y11" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E12" s="10" t="s">
         <v>40</v>
       </c>
@@ -1208,12 +1337,20 @@
       <c r="U12" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="V12" s="16"/>
       <c r="W12" s="9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Y12" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z12" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA12" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M13" s="8" t="s">
         <v>56</v>
       </c>
@@ -1229,12 +1366,20 @@
       <c r="U13" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="V13" s="16"/>
       <c r="W13" s="9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Y13" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z13" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA13" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I14" s="2" t="s">
         <v>41</v>
       </c>
@@ -1258,12 +1403,20 @@
       <c r="U14" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="V14" s="16"/>
       <c r="W14" s="9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Y14" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA14" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="I15" s="5" t="s">
         <v>8</v>
       </c>
@@ -1291,12 +1444,11 @@
       <c r="U15" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="V15" s="16"/>
       <c r="W15" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="I16" s="8" t="s">
         <v>5</v>
       </c>
@@ -1324,7 +1476,6 @@
       <c r="U16" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="V16" s="16"/>
       <c r="W16" s="9" t="s">
         <v>10</v>
       </c>
@@ -1357,7 +1508,6 @@
       <c r="U17" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="V17" s="16"/>
       <c r="W17" s="9" t="s">
         <v>10</v>
       </c>
@@ -1390,7 +1540,6 @@
       <c r="U18" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="V18" s="16"/>
       <c r="W18" s="9" t="s">
         <v>10</v>
       </c>
@@ -1423,7 +1572,6 @@
       <c r="U19" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="V19" s="16"/>
       <c r="W19" s="9" t="s">
         <v>10</v>
       </c>
@@ -1459,7 +1607,6 @@
       <c r="U20" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="V20" s="16"/>
       <c r="W20" s="9" t="s">
         <v>10</v>
       </c>
@@ -1486,7 +1633,7 @@
       <c r="U21" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="V21" s="17" t="s">
+      <c r="V21" t="s">
         <v>12</v>
       </c>
       <c r="W21" s="9" t="s">
@@ -1511,7 +1658,7 @@
       <c r="Q22" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="R22" s="17" t="s">
+      <c r="R22" t="s">
         <v>12</v>
       </c>
       <c r="S22" s="9" t="s">
@@ -1520,7 +1667,7 @@
       <c r="U22" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="V22" s="16" t="s">
+      <c r="V22" t="s">
         <v>12</v>
       </c>
       <c r="W22" s="9" t="s">
@@ -1558,7 +1705,7 @@
       <c r="U23" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="V23" s="16" t="s">
+      <c r="V23" t="s">
         <v>12</v>
       </c>
       <c r="W23" s="9" t="s">
@@ -1596,14 +1743,14 @@
       <c r="U24" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="V24" s="16" t="s">
+      <c r="V24" t="s">
         <v>12</v>
       </c>
       <c r="W24" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="9:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="9:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I25" s="8" t="s">
         <v>18</v>
       </c>
@@ -1613,7 +1760,7 @@
       <c r="M25" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="N25" s="17" t="s">
+      <c r="N25" t="s">
         <v>12</v>
       </c>
       <c r="O25" s="9" t="s">
@@ -1622,7 +1769,7 @@
       <c r="U25" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="V25" s="16" t="s">
+      <c r="V25" t="s">
         <v>12</v>
       </c>
       <c r="W25" s="9" t="s">
@@ -1645,10 +1792,15 @@
       <c r="O26" s="9" t="s">
         <v>11</v>
       </c>
+      <c r="Q26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="R26" s="3"/>
+      <c r="S26" s="4"/>
       <c r="U26" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="V26" s="16" t="s">
+      <c r="V26" t="s">
         <v>12</v>
       </c>
       <c r="W26" s="9" t="s">
@@ -1674,10 +1826,19 @@
       <c r="O27" s="12" t="s">
         <v>10</v>
       </c>
+      <c r="Q27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R27" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="S27" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="U27" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="V27" s="16" t="s">
+      <c r="V27" t="s">
         <v>12</v>
       </c>
       <c r="W27" s="9" t="s">
@@ -1694,10 +1855,19 @@
       <c r="K28" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="Q28" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="R28" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="S28" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="U28" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="V28" s="17" t="s">
+      <c r="V28" t="s">
         <v>12</v>
       </c>
       <c r="W28" s="9" t="s">
@@ -1712,10 +1882,17 @@
       <c r="K29" s="12" t="s">
         <v>11</v>
       </c>
+      <c r="Q29" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="R29" s="16"/>
+      <c r="S29" s="20" t="s">
+        <v>64</v>
+      </c>
       <c r="U29" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="V29" s="16" t="s">
+      <c r="V29" t="s">
         <v>12</v>
       </c>
       <c r="W29" s="9" t="s">
@@ -1723,6 +1900,15 @@
       </c>
     </row>
     <row r="30" spans="9:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q30" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="R30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="S30" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="U30" s="10" t="s">
         <v>62</v>
       </c>
@@ -1733,7 +1919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="9:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="9:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I31" s="2" t="s">
         <v>26</v>
       </c>
@@ -1750,8 +1936,13 @@
       <c r="K32" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="U32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="V32" s="3"/>
+      <c r="W32" s="4"/>
+    </row>
+    <row r="33" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I33" s="8" t="s">
         <v>5</v>
       </c>
@@ -1761,24 +1952,49 @@
       <c r="K33" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="U33" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="V33" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="W33" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I34" s="8" t="s">
         <v>26</v>
       </c>
       <c r="K34" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="35" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="U34" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="V34" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="W34" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="9:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I35" s="8" t="s">
         <v>27</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="U35" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="V35" s="11"/>
+      <c r="W35" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="9:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I36" s="8" t="s">
         <v>14</v>
       </c>
@@ -1786,31 +2002,54 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="9:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I37" s="8" t="s">
         <v>28</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="U37" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="V37" s="3"/>
+      <c r="W37" s="4"/>
+    </row>
+    <row r="38" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I38" s="8" t="s">
         <v>29</v>
       </c>
       <c r="K38" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="U38" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="V38" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="W38" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I39" s="8" t="s">
         <v>30</v>
       </c>
       <c r="K39" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="U39" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="V39" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="W39" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="9:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I40" s="8" t="s">
         <v>19</v>
       </c>
@@ -1820,8 +2059,15 @@
       <c r="K40" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="41" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="U40" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="V40" s="11"/>
+      <c r="W40" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I41" s="8" t="s">
         <v>21</v>
       </c>
@@ -1832,7 +2078,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="9:11" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="9:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I42" s="10" t="s">
         <v>25</v>
       </c>
@@ -1841,46 +2087,45 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="9:11" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="44" spans="9:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="9:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I44" s="2" t="s">
         <v>31</v>
       </c>
       <c r="J44" s="3"/>
       <c r="K44" s="4"/>
     </row>
-    <row r="45" spans="9:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I45" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J45" s="15" t="s">
+      <c r="J45" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K45" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="9:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I46" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J46" s="16" t="s">
+      <c r="J46" t="s">
         <v>6</v>
       </c>
       <c r="K46" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="9:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I47" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="J47" s="16"/>
       <c r="K47" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="9:11" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="9:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I48" s="10" t="s">
         <v>70</v>
       </c>
@@ -2072,18 +2317,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2106,18 +2351,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EF9DAF2-2BB7-423F-B396-DB7EFC3ABE13}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39FBB235-1553-4865-A28D-01E1A5E87283}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39FBB235-1553-4865-A28D-01E1A5E87283}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EF9DAF2-2BB7-423F-B396-DB7EFC3ABE13}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>